<commit_message>
refactor: rename column Transportadora to Importadora
</commit_message>
<xml_diff>
--- a/public/Templates/transferencia.xlsx
+++ b/public/Templates/transferencia.xlsx
@@ -19,7 +19,7 @@
     <t>Código</t>
   </si>
   <si>
-    <t>Transportadora</t>
+    <t>Importadora</t>
   </si>
   <si>
     <t>Quantidade</t>
@@ -374,17 +374,17 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -411,10 +411,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -653,12 +653,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -935,7 +935,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -962,10 +962,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1214,7 +1214,7 @@
   <sheetFormatPr defaultColWidth="11.1667" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="2" width="11" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.3828" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.3516" style="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="1" customWidth="1"/>
     <col min="5" max="5" width="13.8516" style="1" customWidth="1"/>
     <col min="6" max="6" width="18.5" style="1" customWidth="1"/>

</xml_diff>